<commit_message>
put traits table into plots for DFA
</commit_message>
<xml_diff>
--- a/data/Abund.names.traits.xlsx
+++ b/data/Abund.names.traits.xlsx
@@ -5,25 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristin.marshall/Rprojects/pfx-ichthyo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinmarshall/pfx-ichthyo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E4AB6946-3AA8-524A-8369-F9A1B56994D0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7D9EE4-27F5-A247-964C-5E6E2559642B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8380" yWindow="-27580" windowWidth="33580" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33580" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Abund.names" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="164">
   <si>
     <t>spp</t>
   </si>
@@ -376,40 +373,18 @@
     <t>sprickle</t>
   </si>
   <si>
-    <t>epibenthic, shelf</t>
-  </si>
-  <si>
     <t>pelagic forage</t>
   </si>
   <si>
     <t>early spring</t>
   </si>
   <si>
-    <t>batch spawner</t>
-  </si>
-  <si>
     <t>pelagic</t>
   </si>
   <si>
     <t>16-20</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">demersal, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="3" tint="0.39997558519241921"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>shelf</t>
-    </r>
-  </si>
-  <si>
     <t>benthic forage</t>
   </si>
   <si>
@@ -422,48 +397,10 @@
     <t>20-25</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="3" tint="0.39997558519241921"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pelagic</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="3" tint="0.39994506668294322"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, nearshore shelf</t>
-    </r>
-  </si>
-  <si>
     <t>late winter-early summer</t>
   </si>
   <si>
     <t>30+</t>
-  </si>
-  <si>
-    <t>benthic, shelf, upper slope</t>
   </si>
   <si>
     <r>
@@ -486,9 +423,6 @@
     <t>15-18</t>
   </si>
   <si>
-    <t>benthic, slope</t>
-  </si>
-  <si>
     <t>spring-early summer</t>
   </si>
   <si>
@@ -502,6 +436,96 @@
   </si>
   <si>
     <t>12-14</t>
+  </si>
+  <si>
+    <t>18-20</t>
+  </si>
+  <si>
+    <t>late spring, summer</t>
+  </si>
+  <si>
+    <t>8-10</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>16-18</t>
+  </si>
+  <si>
+    <t>spring-summer</t>
+  </si>
+  <si>
+    <t>winter-early spring</t>
+  </si>
+  <si>
+    <t>late spring</t>
+  </si>
+  <si>
+    <t>late winter-spring</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>late spring-summer</t>
+  </si>
+  <si>
+    <t>summer-fall</t>
+  </si>
+  <si>
+    <t>Habitat</t>
+  </si>
+  <si>
+    <t>Guild</t>
+  </si>
+  <si>
+    <t>Dur.short</t>
+  </si>
+  <si>
+    <t>Larval.Duration.wks</t>
+  </si>
+  <si>
+    <t>Egg.Ecology</t>
+  </si>
+  <si>
+    <t>Spawn.time</t>
+  </si>
+  <si>
+    <t>epibenthic.shelf</t>
+  </si>
+  <si>
+    <t>demersal.shelf</t>
+  </si>
+  <si>
+    <t>benthic.slope</t>
+  </si>
+  <si>
+    <t>benthic.shelf</t>
+  </si>
+  <si>
+    <t>pelagic.slope</t>
+  </si>
+  <si>
+    <t>pelagic.shelf</t>
+  </si>
+  <si>
+    <t>demersal.slope</t>
+  </si>
+  <si>
+    <t>benthic.shelf.upper.slope</t>
+  </si>
+  <si>
+    <t>pelagic.nearshore.shelf</t>
+  </si>
+  <si>
+    <t>demersal.nearshore.shelf</t>
+  </si>
+  <si>
+    <t>benthic.outer.shelf.slope</t>
   </si>
 </sst>
 </file>
@@ -1002,13 +1026,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1065,560 +1093,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="C2" t="str">
-            <v>Pacific sand lance</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>epibenthic, nearshore shelf</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>pelagic forage</v>
-          </cell>
-          <cell r="F2" t="str">
-            <v>autumn, winter</v>
-          </cell>
-          <cell r="H2" t="str">
-            <v>demersal</v>
-          </cell>
-          <cell r="I2" t="str">
-            <v>30+</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3" t="str">
-            <v>blennies</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>demersal, nearshore shelf</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="H3" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4" t="str">
-            <v>Arrowtooth flounder</v>
-          </cell>
-          <cell r="D4" t="str">
-            <v>benthic, slope</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>apex predator</v>
-          </cell>
-          <cell r="F4" t="str">
-            <v>winter</v>
-          </cell>
-          <cell r="H4" t="str">
-            <v>pelagic</v>
-          </cell>
-          <cell r="I4" t="str">
-            <v>20-24</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5" t="str">
-            <v>Gray starsnout poacher</v>
-          </cell>
-          <cell r="D5" t="str">
-            <v>demersal, shelf</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6" t="str">
-            <v>Ronquils</v>
-          </cell>
-          <cell r="D6" t="str">
-            <v>demersal, slope</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="H6" t="str">
-            <v>demersal</v>
-          </cell>
-          <cell r="I6" t="str">
-            <v>20-25</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7" t="str">
-            <v>Dwarf wrymouth</v>
-          </cell>
-          <cell r="D7" t="str">
-            <v>demersal, shelf</v>
-          </cell>
-          <cell r="E7" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="F7" t="str">
-            <v>spring, summer</v>
-          </cell>
-          <cell r="H7" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8" t="str">
-            <v>Walleye pollock</v>
-          </cell>
-          <cell r="D8" t="str">
-            <v>epibenthic, shelf</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>pelagic forage</v>
-          </cell>
-          <cell r="F8" t="str">
-            <v>early spring</v>
-          </cell>
-          <cell r="G8" t="str">
-            <v>batch spawner</v>
-          </cell>
-          <cell r="H8" t="str">
-            <v>pelagic</v>
-          </cell>
-          <cell r="I8" t="str">
-            <v>16-20</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9" t="str">
-            <v>Pacific cod</v>
-          </cell>
-          <cell r="D9" t="str">
-            <v>epibenthic, shelf</v>
-          </cell>
-          <cell r="E9" t="str">
-            <v>apex predator</v>
-          </cell>
-          <cell r="F9" t="str">
-            <v>early spring</v>
-          </cell>
-          <cell r="G9" t="str">
-            <v>batch spawner</v>
-          </cell>
-          <cell r="H9" t="str">
-            <v>demersal</v>
-          </cell>
-          <cell r="I9" t="str">
-            <v>12-14</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10" t="str">
-            <v>Kelp greenling</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>demersal, nearshore shelf</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>forage (benthic, pelagic?)</v>
-          </cell>
-          <cell r="F10" t="str">
-            <v>autumn</v>
-          </cell>
-          <cell r="H10" t="str">
-            <v>demersal</v>
-          </cell>
-          <cell r="I10" t="str">
-            <v>30+</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11" t="str">
-            <v>Flathead sole</v>
-          </cell>
-          <cell r="D11" t="str">
-            <v>benthic, shelf, upper slope</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>pelagic forage</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>early spring</v>
-          </cell>
-          <cell r="H11" t="str">
-            <v>pelagic</v>
-          </cell>
-          <cell r="I11" t="str">
-            <v>15-18</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12" t="str">
-            <v>Pacific halibut</v>
-          </cell>
-          <cell r="D12" t="str">
-            <v>benthic, slope</v>
-          </cell>
-          <cell r="E12" t="str">
-            <v>apex predator</v>
-          </cell>
-          <cell r="F12" t="str">
-            <v>winter</v>
-          </cell>
-          <cell r="G12" t="str">
-            <v>batch spawner</v>
-          </cell>
-          <cell r="H12" t="str">
-            <v>demersal</v>
-          </cell>
-          <cell r="I12" t="str">
-            <v>20-24</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13" t="str">
-            <v>Sculpins A</v>
-          </cell>
-          <cell r="D13" t="str">
-            <v>demersal, nearshore shelf</v>
-          </cell>
-          <cell r="E13" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="H13" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14" t="str">
-            <v>Southern rock sole</v>
-          </cell>
-          <cell r="D14" t="str">
-            <v>benthic, shelf</v>
-          </cell>
-          <cell r="E14" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="F14" t="str">
-            <v>late spring, summer</v>
-          </cell>
-          <cell r="G14" t="str">
-            <v>batch spawner</v>
-          </cell>
-          <cell r="H14" t="str">
-            <v>demersal</v>
-          </cell>
-          <cell r="I14" t="str">
-            <v>16-18</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15" t="str">
-            <v>Northern rock sole</v>
-          </cell>
-          <cell r="D15" t="str">
-            <v>benthic, shelf</v>
-          </cell>
-          <cell r="E15" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="F15" t="str">
-            <v>early spring</v>
-          </cell>
-          <cell r="G15" t="str">
-            <v>batch spawner</v>
-          </cell>
-          <cell r="H15" t="str">
-            <v>demersal</v>
-          </cell>
-          <cell r="I15" t="str">
-            <v>18-20</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16" t="str">
-            <v>Daubed shanny</v>
-          </cell>
-          <cell r="D16" t="str">
-            <v>demersal, nearshore shelf</v>
-          </cell>
-          <cell r="E16" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="H16" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17" t="str">
-            <v>Starry flounder</v>
-          </cell>
-          <cell r="D17" t="str">
-            <v>benthic, shelf, upper slope</v>
-          </cell>
-          <cell r="E17" t="str">
-            <v>pelagic forage</v>
-          </cell>
-          <cell r="F17" t="str">
-            <v>late spring, summer</v>
-          </cell>
-          <cell r="H17" t="str">
-            <v>pelagic</v>
-          </cell>
-          <cell r="I17" t="str">
-            <v>8-10</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18" t="str">
-            <v>Whitebarred prickleback</v>
-          </cell>
-          <cell r="D18" t="str">
-            <v>demersal, shelf</v>
-          </cell>
-          <cell r="E18" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="H18" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19" t="str">
-            <v>Northern flashlight fish</v>
-          </cell>
-          <cell r="D19" t="str">
-            <v>pelagic, slope</v>
-          </cell>
-          <cell r="E19" t="str">
-            <v>pelagic forage</v>
-          </cell>
-          <cell r="F19" t="str">
-            <v>winter</v>
-          </cell>
-          <cell r="H19" t="str">
-            <v>pelagic</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20" t="str">
-            <v>Sculpins B</v>
-          </cell>
-          <cell r="D20" t="str">
-            <v>demersal, shelf</v>
-          </cell>
-          <cell r="E20" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="H20" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21" t="str">
-            <v>Rockfish</v>
-          </cell>
-          <cell r="D21" t="str">
-            <v>benthic, slope</v>
-          </cell>
-          <cell r="E21" t="str">
-            <v>pelagic forage</v>
-          </cell>
-          <cell r="F21" t="str">
-            <v>early spring</v>
-          </cell>
-          <cell r="H21" t="str">
-            <v>live bearing</v>
-          </cell>
-          <cell r="I21" t="str">
-            <v>20-24</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22" t="str">
-            <v>Northern lampfish</v>
-          </cell>
-          <cell r="D22" t="str">
-            <v>pelagic, slope</v>
-          </cell>
-          <cell r="E22" t="str">
-            <v>pelagic forage</v>
-          </cell>
-          <cell r="F22" t="str">
-            <v>winter</v>
-          </cell>
-          <cell r="H22" t="str">
-            <v>pelagic</v>
-          </cell>
-          <cell r="I22" t="str">
-            <v>30+</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23" t="str">
-            <v>prowfish</v>
-          </cell>
-          <cell r="D23" t="str">
-            <v>demersal, slope</v>
-          </cell>
-          <cell r="E23" t="str">
-            <v>benthic forage</v>
-          </cell>
-          <cell r="H23" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25" t="str">
-            <v>spinycheek starsnout</v>
-          </cell>
-          <cell r="D25" t="str">
-            <v>demersal, shelf</v>
-          </cell>
-          <cell r="F25" t="str">
-            <v>??</v>
-          </cell>
-          <cell r="H25" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26" t="str">
-            <v>Pacific blacksmelt</v>
-          </cell>
-          <cell r="D26" t="str">
-            <v>pelagic, slope</v>
-          </cell>
-          <cell r="F26" t="str">
-            <v>spring (feb-march)</v>
-          </cell>
-          <cell r="H26" t="str">
-            <v>pelagic</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27" t="str">
-            <v>Pacific herring</v>
-          </cell>
-          <cell r="D27" t="str">
-            <v>pelagic, shelf</v>
-          </cell>
-          <cell r="F27" t="str">
-            <v>late spring</v>
-          </cell>
-          <cell r="H27" t="str">
-            <v>demersal</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28" t="str">
-            <v>Rex sole</v>
-          </cell>
-          <cell r="D28" t="str">
-            <v>demersal</v>
-          </cell>
-          <cell r="F28" t="str">
-            <v>spring</v>
-          </cell>
-          <cell r="H28" t="str">
-            <v>pelagic</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29" t="str">
-            <v>Butter sole</v>
-          </cell>
-          <cell r="D29" t="str">
-            <v>benthic, shelf</v>
-          </cell>
-          <cell r="F29" t="str">
-            <v>early spring</v>
-          </cell>
-          <cell r="H29" t="str">
-            <v>pelagic</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30" t="str">
-            <v>Northern smoothtounge</v>
-          </cell>
-          <cell r="H30" t="str">
-            <v>pelagic</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31" t="str">
-            <v>slipskin snailfish</v>
-          </cell>
-          <cell r="D31" t="str">
-            <v>slope</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32" t="str">
-            <v>longsnout prickleback</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33" t="str">
-            <v>snake prickleback</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34" t="str">
-            <v>capelin</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35" t="str">
-            <v>dover sole</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36" t="str">
-            <v>deepwater sculpin</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37" t="str">
-            <v>lingcod</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39" t="str">
-            <v>Alaska plaice</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40" t="str">
-            <v>sturgeon poacher</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41" t="str">
-            <v>Puget Sound sculpin</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42" t="str">
-            <v>sculpins C</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1918,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:J7"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1929,12 +1403,13 @@
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1944,8 +1419,26 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="D1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1955,9 +1448,8 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(B2,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>epibenthic, shelf</v>
+      <c r="D2" t="s">
+        <v>153</v>
       </c>
       <c r="E2" t="s">
         <v>117</v>
@@ -1968,17 +1460,15 @@
       <c r="G2" t="s">
         <v>119</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="I2" t="str">
+        <f>LEFT(H2,2)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1988,27 +1478,27 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="str">
-        <f>VLOOKUP(B3,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, slope</v>
+      <c r="D3" t="s">
+        <v>154</v>
       </c>
       <c r="E3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" t="s">
         <v>123</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" t="s">
-        <v>126</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="19">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I41" si="0">LEFT(H3,2)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="19">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2018,27 +1508,27 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="str">
-        <f>VLOOKUP(B4,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>benthic, shelf, upper slope</v>
-      </c>
-      <c r="E4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>132</v>
+      <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" t="s">
+        <v>118</v>
       </c>
       <c r="G4" t="s">
         <v>119</v>
       </c>
-      <c r="I4" t="s">
-        <v>121</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="19">
+      <c r="H4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2048,27 +1538,27 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="str">
-        <f>VLOOKUP(B5,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>epibenthic, nearshore shelf</v>
+      <c r="D5" t="s">
+        <v>161</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2078,27 +1568,27 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="str">
-        <f>VLOOKUP(B6,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>benthic, slope</v>
+      <c r="D6" t="s">
+        <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I6" t="s">
-        <v>136</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>117</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2108,30 +1598,27 @@
       <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="str">
-        <f>VLOOKUP(B7,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>epibenthic, shelf</v>
-      </c>
-      <c r="E7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>138</v>
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" t="s">
+        <v>118</v>
       </c>
       <c r="G7" t="s">
-        <v>119</v>
-      </c>
-      <c r="H7" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>123</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2141,12 +1628,27 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="str">
-        <f>VLOOKUP(B8,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>benthic, shelf</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="D8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2156,12 +1658,26 @@
       <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="str">
-        <f>VLOOKUP(B9,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>benthic, shelf, upper slope</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="D9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2171,12 +1687,27 @@
       <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="str">
-        <f>VLOOKUP(B10,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, nearshore shelf</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="D10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2186,12 +1717,27 @@
       <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="str">
-        <f>VLOOKUP(B11,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>pelagic, slope</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="D11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2201,12 +1747,27 @@
       <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="str">
-        <f>VLOOKUP(B12,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>benthic, shelf</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="D12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -2216,12 +1777,27 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="str">
-        <f>VLOOKUP(B13,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>benthic, slope</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="D13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2231,12 +1807,27 @@
       <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="str">
-        <f>VLOOKUP(B14,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, nearshore shelf</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="D14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2246,12 +1837,26 @@
       <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="str">
-        <f>VLOOKUP(B15,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>benthic, shelf</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="D15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2261,12 +1866,27 @@
       <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="str">
-        <f>VLOOKUP(B16,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, shelf</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2276,12 +1896,27 @@
       <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="D17" t="str">
-        <f>VLOOKUP(B17,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, shelf</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2291,12 +1926,27 @@
       <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="str">
-        <f>VLOOKUP(B18,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, shelf</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2306,12 +1956,27 @@
       <c r="C19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="str">
-        <f>VLOOKUP(B19,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, nearshore shelf</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" t="s">
+        <v>123</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2321,12 +1986,27 @@
       <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="str">
-        <f>VLOOKUP(B20,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, nearshore shelf</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="19">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -2336,12 +2016,27 @@
       <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="str">
-        <f>VLOOKUP(B21,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -2351,12 +2046,26 @@
       <c r="C22" t="s">
         <v>62</v>
       </c>
-      <c r="D22" t="str">
-        <f>VLOOKUP(B22,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>slope</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2366,12 +2075,27 @@
       <c r="C23" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="str">
-        <f>VLOOKUP(B23,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>benthic, slope</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D23" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -2381,12 +2105,27 @@
       <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="D24">
-        <f>VLOOKUP(B24,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2396,12 +2135,27 @@
       <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="D25" t="str">
-        <f>VLOOKUP(B25,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, shelf</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" t="s">
+        <v>123</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2411,12 +2165,27 @@
       <c r="C26" t="s">
         <v>74</v>
       </c>
-      <c r="D26">
-        <f>VLOOKUP(B26,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2426,12 +2195,26 @@
       <c r="C27" t="s">
         <v>77</v>
       </c>
-      <c r="D27">
-        <f>VLOOKUP(B27,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -2441,12 +2224,27 @@
       <c r="C28" t="s">
         <v>80</v>
       </c>
-      <c r="D28" t="str">
-        <f>VLOOKUP(B28,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>pelagic, shelf</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" t="s">
+        <v>158</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" t="s">
+        <v>142</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -2456,12 +2254,27 @@
       <c r="C29" t="s">
         <v>83</v>
       </c>
-      <c r="D29" t="str">
-        <f>VLOOKUP(B29,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>demersal, slope</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" t="s">
+        <v>159</v>
+      </c>
+      <c r="E29" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" t="s">
+        <v>123</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -2471,12 +2284,27 @@
       <c r="C30" t="s">
         <v>85</v>
       </c>
-      <c r="D30" t="e">
-        <f>VLOOKUP(B30,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="D30" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -2486,12 +2314,27 @@
       <c r="C31" t="s">
         <v>88</v>
       </c>
-      <c r="D31" t="e">
-        <f>VLOOKUP(B31,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2501,12 +2344,27 @@
       <c r="C32" t="s">
         <v>90</v>
       </c>
-      <c r="D32">
-        <f>VLOOKUP(B32,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="D32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="19">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -2516,12 +2374,27 @@
       <c r="C33" t="s">
         <v>92</v>
       </c>
-      <c r="D33">
-        <f>VLOOKUP(B33,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="D33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2531,12 +2404,27 @@
       <c r="C34" t="s">
         <v>95</v>
       </c>
-      <c r="D34">
-        <f>VLOOKUP(B34,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="D34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>96</v>
       </c>
@@ -2546,12 +2434,27 @@
       <c r="C35" t="s">
         <v>98</v>
       </c>
-      <c r="D35" t="e">
-        <f>VLOOKUP(B35,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="D35" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" t="s">
+        <v>123</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -2561,12 +2464,27 @@
       <c r="C36" t="s">
         <v>101</v>
       </c>
-      <c r="D36">
-        <f>VLOOKUP(B36,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="D36" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>102</v>
       </c>
@@ -2576,12 +2494,27 @@
       <c r="C37" t="s">
         <v>104</v>
       </c>
-      <c r="D37" t="e">
-        <f>VLOOKUP(B37,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="D37" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" t="s">
+        <v>138</v>
+      </c>
+      <c r="G37" t="s">
+        <v>119</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -2591,12 +2524,27 @@
       <c r="C38" t="s">
         <v>107</v>
       </c>
-      <c r="D38" t="e">
-        <f>VLOOKUP(B38,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" t="s">
+        <v>119</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -2606,12 +2554,27 @@
       <c r="C39" t="s">
         <v>110</v>
       </c>
-      <c r="D39">
-        <f>VLOOKUP(B39,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="D39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>111</v>
       </c>
@@ -2621,12 +2584,27 @@
       <c r="C40" t="s">
         <v>113</v>
       </c>
-      <c r="D40">
-        <f>VLOOKUP(B40,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="D40" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -2636,9 +2614,24 @@
       <c r="C41" t="s">
         <v>116</v>
       </c>
-      <c r="D41">
-        <f>VLOOKUP(B41,[1]Sheet1!$C$2:$I$42, 2,FALSE)</f>
-        <v>0</v>
+      <c r="D41" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added life history train tables, new plots for cluster analysis
</commit_message>
<xml_diff>
--- a/data/Abund.names.traits.xlsx
+++ b/data/Abund.names.traits.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinmarshall/pfx-ichthyo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristin.marshall/Rprojects/pfx-ichthyo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7D9EE4-27F5-A247-964C-5E6E2559642B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C007DE51-5E87-3140-A372-7BF4700158D0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33580" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="580" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Abund.names" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="160">
   <si>
     <t>spp</t>
   </si>
@@ -388,16 +388,10 @@
     <t>benthic forage</t>
   </si>
   <si>
-    <t>late spring- summer</t>
-  </si>
-  <si>
     <t>demersal</t>
   </si>
   <si>
     <t>20-25</t>
-  </si>
-  <si>
-    <t>late winter-early summer</t>
   </si>
   <si>
     <t>30+</t>
@@ -423,9 +417,6 @@
     <t>15-18</t>
   </si>
   <si>
-    <t>spring-early summer</t>
-  </si>
-  <si>
     <t>live bearing</t>
   </si>
   <si>
@@ -441,9 +432,6 @@
     <t>18-20</t>
   </si>
   <si>
-    <t>late spring, summer</t>
-  </si>
-  <si>
     <t>8-10</t>
   </si>
   <si>
@@ -456,45 +444,24 @@
     <t>16-18</t>
   </si>
   <si>
-    <t>spring-summer</t>
-  </si>
-  <si>
-    <t>winter-early spring</t>
-  </si>
-  <si>
     <t>late spring</t>
   </si>
   <si>
-    <t>late winter-spring</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>late spring-summer</t>
-  </si>
-  <si>
-    <t>summer-fall</t>
-  </si>
-  <si>
     <t>Habitat</t>
   </si>
   <si>
     <t>Guild</t>
   </si>
   <si>
-    <t>Dur.short</t>
-  </si>
-  <si>
     <t>Larval.Duration.wks</t>
   </si>
   <si>
     <t>Egg.Ecology</t>
   </si>
   <si>
-    <t>Spawn.time</t>
-  </si>
-  <si>
     <t>epibenthic.shelf</t>
   </si>
   <si>
@@ -526,6 +493,27 @@
   </si>
   <si>
     <t>benthic.outer.shelf.slope</t>
+  </si>
+  <si>
+    <t>ubiquitous</t>
+  </si>
+  <si>
+    <t>north</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Spawn.short</t>
+  </si>
+  <si>
+    <t>late winter</t>
+  </si>
+  <si>
+    <t>summer</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1383,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="I1" sqref="D1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1405,7 +1393,6 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1420,22 +1407,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>152</v>
+        <v>139</v>
+      </c>
+      <c r="F1" t="s">
+        <v>157</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>149</v>
+        <v>140</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1449,7 +1436,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E2" t="s">
         <v>117</v>
@@ -1463,9 +1450,8 @@
       <c r="H2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I2" t="str">
-        <f>LEFT(H2,2)</f>
-        <v>16</v>
+      <c r="I2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1479,23 +1465,22 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>122</v>
+      <c r="F3" t="s">
+        <v>136</v>
       </c>
       <c r="G3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I41" si="0">LEFT(H3,2)</f>
-        <v>20</v>
+      <c r="I3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="19">
@@ -1509,10 +1494,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F4" t="s">
         <v>118</v>
@@ -1521,14 +1506,13 @@
         <v>119</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19">
+        <v>126</v>
+      </c>
+      <c r="I4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1539,23 +1523,22 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E5" t="s">
         <v>117</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>125</v>
+      <c r="F5" t="s">
+        <v>158</v>
       </c>
       <c r="G5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>124</v>
+      </c>
+      <c r="I5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1569,23 +1552,22 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E6" t="s">
         <v>117</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>129</v>
+      <c r="F6" t="s">
+        <v>133</v>
       </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>128</v>
+      </c>
+      <c r="I6" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1599,23 +1581,22 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F7" t="s">
         <v>118</v>
       </c>
       <c r="G7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I7" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1629,7 +1610,7 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
         <v>121</v>
@@ -1638,14 +1619,13 @@
         <v>118</v>
       </c>
       <c r="G8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <v>131</v>
+      </c>
+      <c r="I8" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1659,22 +1639,22 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E9" t="s">
         <v>117</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G9" t="s">
         <v>119</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
+        <v>132</v>
+      </c>
+      <c r="I9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1688,23 +1668,22 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E10" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G10" t="s">
-        <v>123</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="I10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1718,23 +1697,22 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
         <v>117</v>
       </c>
       <c r="F11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G11" t="s">
         <v>119</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>124</v>
+      </c>
+      <c r="I11" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1748,23 +1726,22 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E12" t="s">
         <v>121</v>
       </c>
       <c r="F12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G12" t="s">
-        <v>123</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="I12" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1778,23 +1755,22 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G13" t="s">
         <v>119</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>128</v>
+      </c>
+      <c r="I13" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1808,23 +1784,22 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E14" t="s">
         <v>121</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>129</v>
+      <c r="F14" t="s">
+        <v>133</v>
       </c>
       <c r="G14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I14" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1838,7 +1813,7 @@
         <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>121</v>
@@ -1850,10 +1825,10 @@
         <v>119</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="I15">
-        <v>8</v>
+        <v>132</v>
+      </c>
+      <c r="I15" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1867,23 +1842,22 @@
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E16" t="s">
         <v>121</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>137</v>
+      <c r="F16" t="s">
+        <v>133</v>
       </c>
       <c r="G16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I16" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1897,23 +1871,22 @@
         <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E17" t="s">
         <v>121</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I17" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1927,23 +1900,22 @@
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E18" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>137</v>
+      <c r="F18" t="s">
+        <v>133</v>
       </c>
       <c r="G18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <v>126</v>
+      </c>
+      <c r="I18" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1957,23 +1929,22 @@
         <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>141</v>
+      <c r="F19" t="s">
+        <v>134</v>
       </c>
       <c r="G19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>124</v>
+      </c>
+      <c r="I19" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1987,26 +1958,25 @@
         <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E20" t="s">
         <v>121</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>137</v>
+      <c r="F20" t="s">
+        <v>133</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="19">
+        <v>128</v>
+      </c>
+      <c r="I20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -2017,23 +1987,22 @@
         <v>59</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F21" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G21" t="s">
         <v>119</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>124</v>
+      </c>
+      <c r="I21" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2047,22 +2016,22 @@
         <v>62</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>142</v>
+      <c r="F22" t="s">
+        <v>136</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="I22">
-        <v>8</v>
+        <v>132</v>
+      </c>
+      <c r="I22" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2076,23 +2045,22 @@
         <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F23" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>128</v>
+      </c>
+      <c r="I23" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2106,23 +2074,22 @@
         <v>68</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>129</v>
+      <c r="F24" t="s">
+        <v>133</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>119</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>124</v>
+      </c>
+      <c r="I24" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2136,23 +2103,22 @@
         <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E25" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" t="s">
+        <v>133</v>
+      </c>
+      <c r="G25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G25" t="s">
-        <v>123</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>NA</v>
+      <c r="I25" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2166,23 +2132,22 @@
         <v>74</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>137</v>
+      <c r="F26" t="s">
+        <v>133</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I26" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I26" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2196,22 +2161,22 @@
         <v>77</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>145</v>
+      <c r="F27" t="s">
+        <v>136</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>119</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="I27">
-        <v>8</v>
+        <v>132</v>
+      </c>
+      <c r="I27" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2225,23 +2190,22 @@
         <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>117</v>
       </c>
       <c r="F28" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I28" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2255,23 +2219,22 @@
         <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="E29" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>137</v>
+      <c r="F29" t="s">
+        <v>133</v>
       </c>
       <c r="G29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="I29" t="str">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="I29" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2285,23 +2248,22 @@
         <v>85</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>125</v>
+      <c r="F30" t="s">
+        <v>158</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I30" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2315,23 +2277,22 @@
         <v>88</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>141</v>
+      <c r="F31" t="s">
+        <v>134</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>119</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I31" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I31" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2345,26 +2306,25 @@
         <v>90</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
+      </c>
+      <c r="F32" t="s">
+        <v>158</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I32" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="19">
+        <v>130</v>
+      </c>
+      <c r="I32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -2375,23 +2335,22 @@
         <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>146</v>
+      <c r="F33" t="s">
+        <v>159</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I33" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>124</v>
+      </c>
+      <c r="I33" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2405,23 +2364,22 @@
         <v>95</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" t="s">
+        <v>133</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I34" t="s">
         <v>154</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="I34" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2435,23 +2393,22 @@
         <v>98</v>
       </c>
       <c r="D35" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>137</v>
+      <c r="F35" t="s">
+        <v>133</v>
       </c>
       <c r="G35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I35" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I35" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2465,23 +2422,22 @@
         <v>101</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>137</v>
+      <c r="F36" t="s">
+        <v>133</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I36" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I36" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2495,23 +2451,22 @@
         <v>104</v>
       </c>
       <c r="D37" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E37" t="s">
         <v>117</v>
       </c>
       <c r="F37" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G37" t="s">
         <v>119</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I37" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>124</v>
+      </c>
+      <c r="I37" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2525,23 +2480,22 @@
         <v>107</v>
       </c>
       <c r="D38" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>141</v>
+      <c r="F38" t="s">
+        <v>134</v>
       </c>
       <c r="G38" t="s">
         <v>119</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I38" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I38" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2555,23 +2509,22 @@
         <v>110</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>137</v>
+      <c r="F39" t="s">
+        <v>133</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I39" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I39" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2585,23 +2538,22 @@
         <v>113</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>137</v>
+      <c r="F40" t="s">
+        <v>133</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I40" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I40" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2615,26 +2567,26 @@
         <v>116</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>143</v>
+      <c r="F41" t="s">
+        <v>158</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I41" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="I41" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>